<commit_message>
Logs for dz4z2.cu added.
</commit_message>
<xml_diff>
--- a/CUDA/racunanje_ubrzanja_programa_cuda.xlsx
+++ b/CUDA/racunanje_ubrzanja_programa_cuda.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saren\OneDrive\Documents\ETF\7. semestar\Multiprocesorski sistemi\GitHub_Domaci\Multiprocessing_Systems\CUDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6CF7BCC-C7A8-42D8-A612-C2EE83C5843A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C969194B-B5EE-4145-A427-CC97F84109FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{E700D36A-9AEC-48B1-B431-3A7C21838328}"/>
   </bookViews>
@@ -264,6 +264,24 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -279,23 +297,14 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -306,13 +315,10 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -323,12 +329,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -653,16 +653,16 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
@@ -694,28 +694,28 @@
       <c r="A3" s="1">
         <v>4.0029999999999996E-3</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="7">
         <f>AVERAGE(A3:A7)</f>
         <v>3.9849999999999998E-3</v>
       </c>
       <c r="C3" s="1">
         <v>1.0662E-2</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="7">
         <f>AVERAGE(C3:C7)</f>
         <v>1.0530999999999999E-2</v>
       </c>
       <c r="E3" s="1">
         <v>0.22844900000000001</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="7">
         <f>AVERAGE(E3:E7)</f>
         <v>0.21360760000000001</v>
       </c>
       <c r="G3" s="1">
         <v>4.5852110000000001</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="8">
         <f>AVERAGE(G3:G7)</f>
         <v>4.6139513999999995</v>
       </c>
@@ -724,89 +724,89 @@
       <c r="A4" s="1">
         <v>3.9899999999999996E-3</v>
       </c>
-      <c r="B4" s="12"/>
+      <c r="B4" s="7"/>
       <c r="C4" s="1">
         <v>1.0253999999999999E-2</v>
       </c>
-      <c r="D4" s="12"/>
+      <c r="D4" s="7"/>
       <c r="E4" s="1">
         <v>0.19584399999999999</v>
       </c>
-      <c r="F4" s="12"/>
+      <c r="F4" s="7"/>
       <c r="G4" s="1">
         <v>4.7025360000000003</v>
       </c>
-      <c r="H4" s="14"/>
+      <c r="H4" s="9"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4.1009999999999996E-3</v>
       </c>
-      <c r="B5" s="12"/>
+      <c r="B5" s="7"/>
       <c r="C5" s="1">
         <v>1.0397999999999999E-2</v>
       </c>
-      <c r="D5" s="12"/>
+      <c r="D5" s="7"/>
       <c r="E5" s="1">
         <v>0.20313800000000001</v>
       </c>
-      <c r="F5" s="12"/>
+      <c r="F5" s="7"/>
       <c r="G5" s="1">
         <v>4.608962</v>
       </c>
-      <c r="H5" s="14"/>
+      <c r="H5" s="9"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>3.9529999999999999E-3</v>
       </c>
-      <c r="B6" s="12"/>
+      <c r="B6" s="7"/>
       <c r="C6" s="1">
         <v>1.0951000000000001E-2</v>
       </c>
-      <c r="D6" s="12"/>
+      <c r="D6" s="7"/>
       <c r="E6" s="1">
         <v>0.19843</v>
       </c>
-      <c r="F6" s="12"/>
+      <c r="F6" s="7"/>
       <c r="G6" s="1">
         <v>4.6466500000000002</v>
       </c>
-      <c r="H6" s="14"/>
+      <c r="H6" s="9"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>3.8779999999999999E-3</v>
       </c>
-      <c r="B7" s="12"/>
+      <c r="B7" s="7"/>
       <c r="C7" s="1">
         <v>1.039E-2</v>
       </c>
-      <c r="D7" s="12"/>
+      <c r="D7" s="7"/>
       <c r="E7" s="1">
         <v>0.242177</v>
       </c>
-      <c r="F7" s="12"/>
+      <c r="F7" s="7"/>
       <c r="G7" s="1">
         <v>4.5263980000000004</v>
       </c>
-      <c r="H7" s="15"/>
+      <c r="H7" s="10"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
@@ -850,44 +850,44 @@
       <c r="A11" s="3">
         <v>2.7099999999999997E-4</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="11">
         <f>AVERAGE(A11:A15)</f>
         <v>2.7240000000000001E-4</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="15">
         <f>B3/B11</f>
         <v>14.629221732745961</v>
       </c>
       <c r="D11" s="3">
         <v>4.4000000000000002E-4</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="11">
         <f>AVERAGE(D11:D15)</f>
         <v>4.3960000000000006E-4</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="12">
         <f>D3/E11</f>
         <v>23.955868971792533</v>
       </c>
       <c r="G11" s="3">
         <v>3.333E-3</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="11">
         <f>AVERAGE(G11:G15)</f>
         <v>3.3340000000000002E-3</v>
       </c>
-      <c r="I11" s="6">
+      <c r="I11" s="12">
         <f>F3/H11</f>
         <v>64.069466106778648</v>
       </c>
       <c r="J11" s="3">
         <v>8.0574999999999994E-2</v>
       </c>
-      <c r="K11" s="5">
+      <c r="K11" s="11">
         <f>AVERAGE(J11:J15)</f>
         <v>8.0560199999999998E-2</v>
       </c>
-      <c r="L11" s="6">
+      <c r="L11" s="12">
         <f>H3/K11</f>
         <v>57.273335964905741</v>
       </c>
@@ -896,98 +896,92 @@
       <c r="A12" s="3">
         <v>2.63E-4</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="9"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="15"/>
       <c r="D12" s="3">
         <v>4.3899999999999999E-4</v>
       </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="7"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="13"/>
       <c r="G12" s="3">
         <v>3.3249999999999998E-3</v>
       </c>
-      <c r="H12" s="5"/>
-      <c r="I12" s="7"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="13"/>
       <c r="J12" s="3">
         <v>8.0686999999999995E-2</v>
       </c>
-      <c r="K12" s="5"/>
-      <c r="L12" s="7"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="13"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>2.7599999999999999E-4</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="9"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="15"/>
       <c r="D13" s="3">
         <v>4.4099999999999999E-4</v>
       </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="7"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="13"/>
       <c r="G13" s="3">
         <v>3.3349999999999999E-3</v>
       </c>
-      <c r="H13" s="5"/>
-      <c r="I13" s="7"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="13"/>
       <c r="J13" s="3">
         <v>8.0436999999999995E-2</v>
       </c>
-      <c r="K13" s="5"/>
-      <c r="L13" s="7"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="13"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>2.7700000000000001E-4</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="9"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="15"/>
       <c r="D14" s="3">
         <v>4.4200000000000001E-4</v>
       </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="7"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="13"/>
       <c r="G14" s="3">
         <v>3.339E-3</v>
       </c>
-      <c r="H14" s="5"/>
-      <c r="I14" s="7"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="13"/>
       <c r="J14" s="3">
         <v>8.0562999999999996E-2</v>
       </c>
-      <c r="K14" s="5"/>
-      <c r="L14" s="7"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="13"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>2.7500000000000002E-4</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="9"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="15"/>
       <c r="D15" s="3">
         <v>4.3600000000000003E-4</v>
       </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="8"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="14"/>
       <c r="G15" s="3">
         <v>3.3379999999999998E-3</v>
       </c>
-      <c r="H15" s="5"/>
-      <c r="I15" s="8"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="14"/>
       <c r="J15" s="3">
         <v>8.0538999999999999E-2</v>
       </c>
-      <c r="K15" s="5"/>
-      <c r="L15" s="8"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A9:L9"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="D3:D7"/>
-    <mergeCell ref="F3:F7"/>
-    <mergeCell ref="H3:H7"/>
     <mergeCell ref="K11:K15"/>
     <mergeCell ref="L11:L15"/>
     <mergeCell ref="B11:B15"/>
@@ -996,6 +990,12 @@
     <mergeCell ref="F11:F15"/>
     <mergeCell ref="H11:H15"/>
     <mergeCell ref="I11:I15"/>
+    <mergeCell ref="A9:L9"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="D3:D7"/>
+    <mergeCell ref="F3:F7"/>
+    <mergeCell ref="H3:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1006,20 +1006,20 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="21"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="18"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
@@ -1043,95 +1043,95 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>1.438E-3</v>
-      </c>
-      <c r="B3" s="12">
+        <v>4.241E-3</v>
+      </c>
+      <c r="B3" s="7">
         <f>AVERAGE(A3:A7)</f>
-        <v>1.9784000000000004E-3</v>
+        <v>2.1372000000000001E-3</v>
       </c>
       <c r="C3" s="1">
-        <v>2.1944000000000002E-2</v>
-      </c>
-      <c r="D3" s="12">
+        <v>2.8559000000000001E-2</v>
+      </c>
+      <c r="D3" s="7">
         <f>AVERAGE(C3:C7)</f>
-        <v>2.25554E-2</v>
+        <v>2.7738400000000003E-2</v>
       </c>
       <c r="E3" s="1">
-        <v>2.4267289999999999</v>
-      </c>
-      <c r="F3" s="12">
+        <v>2.2680989999999999</v>
+      </c>
+      <c r="F3" s="7">
         <f>AVERAGE(E3:E7)</f>
-        <v>2.2378609999999997</v>
+        <v>2.2161198</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>1.317E-3</v>
-      </c>
-      <c r="B4" s="12"/>
+        <v>1.5939999999999999E-3</v>
+      </c>
+      <c r="B4" s="7"/>
       <c r="C4" s="1">
-        <v>2.9302000000000002E-2</v>
-      </c>
-      <c r="D4" s="12"/>
+        <v>2.7979E-2</v>
+      </c>
+      <c r="D4" s="7"/>
       <c r="E4" s="1">
-        <v>1.8761060000000001</v>
-      </c>
-      <c r="F4" s="12"/>
+        <v>2.19848</v>
+      </c>
+      <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>3.32E-3</v>
-      </c>
-      <c r="B5" s="12"/>
+        <v>1.56E-3</v>
+      </c>
+      <c r="B5" s="7"/>
       <c r="C5" s="1">
-        <v>2.3130000000000001E-2</v>
-      </c>
-      <c r="D5" s="12"/>
+        <v>2.3862999999999999E-2</v>
+      </c>
+      <c r="D5" s="7"/>
       <c r="E5" s="1">
-        <v>2.4563670000000002</v>
-      </c>
-      <c r="F5" s="12"/>
+        <v>2.2217060000000002</v>
+      </c>
+      <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>1.47E-3</v>
-      </c>
-      <c r="B6" s="12"/>
+        <v>1.663E-3</v>
+      </c>
+      <c r="B6" s="7"/>
       <c r="C6" s="1">
-        <v>1.6910000000000001E-2</v>
-      </c>
-      <c r="D6" s="12"/>
+        <v>3.1158000000000002E-2</v>
+      </c>
+      <c r="D6" s="7"/>
       <c r="E6" s="1">
-        <v>2.0546519999999999</v>
-      </c>
-      <c r="F6" s="12"/>
+        <v>2.086471</v>
+      </c>
+      <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>2.3470000000000001E-3</v>
-      </c>
-      <c r="B7" s="12"/>
+        <v>1.6280000000000001E-3</v>
+      </c>
+      <c r="B7" s="7"/>
       <c r="C7" s="1">
-        <v>2.1491E-2</v>
-      </c>
-      <c r="D7" s="12"/>
+        <v>2.7133000000000001E-2</v>
+      </c>
+      <c r="D7" s="7"/>
       <c r="E7" s="1">
-        <v>2.375451</v>
-      </c>
-      <c r="F7" s="12"/>
+        <v>2.3058429999999999</v>
+      </c>
+      <c r="F7" s="7"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="18"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="21"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
@@ -1164,120 +1164,120 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
-        <v>6.4700000000000001E-4</v>
-      </c>
-      <c r="B11" s="5">
+        <v>9.5614000000000005E-2</v>
+      </c>
+      <c r="B11" s="11">
         <f>AVERAGE(A11:A15)</f>
-        <v>5.9120000000000006E-4</v>
-      </c>
-      <c r="C11" s="9">
+        <v>8.6125800000000002E-2</v>
+      </c>
+      <c r="C11" s="15">
         <f>B3/B11</f>
-        <v>3.3464140730717187</v>
+        <v>2.4814863838710351E-2</v>
       </c>
       <c r="D11" s="3">
-        <v>3.3813999999999997E-2</v>
-      </c>
-      <c r="E11" s="5">
+        <v>8.5962999999999998E-2</v>
+      </c>
+      <c r="E11" s="11">
         <f>AVERAGE(D11:D15)</f>
-        <v>2.8969399999999999E-2</v>
-      </c>
-      <c r="F11" s="6">
+        <v>8.4431400000000004E-2</v>
+      </c>
+      <c r="F11" s="12">
         <f>D3/E11</f>
-        <v>0.77859396466616504</v>
+        <v>0.32853180214943734</v>
       </c>
       <c r="G11" s="3">
-        <v>1.9461379999999999</v>
-      </c>
-      <c r="H11" s="5">
+        <v>1.0524530000000001</v>
+      </c>
+      <c r="H11" s="11">
         <f>AVERAGE(G11:G15)</f>
-        <v>2.1034044000000001</v>
-      </c>
-      <c r="I11" s="6">
+        <v>1.0546840000000002</v>
+      </c>
+      <c r="I11" s="12">
         <f>F3/H11</f>
-        <v>1.0639233235415879</v>
+        <v>2.1012168573714969</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
-        <v>5.7899999999999998E-4</v>
-      </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="9"/>
+        <v>9.0286000000000005E-2</v>
+      </c>
+      <c r="B12" s="11"/>
+      <c r="C12" s="15"/>
       <c r="D12" s="3">
-        <v>2.0060999999999999E-2</v>
-      </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="7"/>
+        <v>9.2688000000000006E-2</v>
+      </c>
+      <c r="E12" s="11"/>
+      <c r="F12" s="13"/>
       <c r="G12" s="3">
-        <v>2.0668820000000001</v>
-      </c>
-      <c r="H12" s="5"/>
-      <c r="I12" s="7"/>
+        <v>1.049847</v>
+      </c>
+      <c r="H12" s="11"/>
+      <c r="I12" s="13"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
-        <v>5.1500000000000005E-4</v>
-      </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="9"/>
+        <v>9.1924000000000006E-2</v>
+      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="15"/>
       <c r="D13" s="3">
-        <v>2.4271999999999998E-2</v>
-      </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="7"/>
+        <v>8.2306000000000004E-2</v>
+      </c>
+      <c r="E13" s="11"/>
+      <c r="F13" s="13"/>
       <c r="G13" s="3">
-        <v>2.3161109999999998</v>
-      </c>
-      <c r="H13" s="5"/>
-      <c r="I13" s="7"/>
+        <v>1.0593520000000001</v>
+      </c>
+      <c r="H13" s="11"/>
+      <c r="I13" s="13"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
-        <v>5.8100000000000003E-4</v>
-      </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="9"/>
+        <v>8.3705000000000002E-2</v>
+      </c>
+      <c r="B14" s="11"/>
+      <c r="C14" s="15"/>
       <c r="D14" s="3">
-        <v>4.6851999999999998E-2</v>
-      </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="7"/>
+        <v>8.0946000000000004E-2</v>
+      </c>
+      <c r="E14" s="11"/>
+      <c r="F14" s="13"/>
       <c r="G14" s="3">
-        <v>1.861777</v>
-      </c>
-      <c r="H14" s="5"/>
-      <c r="I14" s="7"/>
+        <v>1.058303</v>
+      </c>
+      <c r="H14" s="11"/>
+      <c r="I14" s="13"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
-        <v>6.3400000000000001E-4</v>
-      </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="9"/>
+        <v>6.9099999999999995E-2</v>
+      </c>
+      <c r="B15" s="11"/>
+      <c r="C15" s="15"/>
       <c r="D15" s="3">
-        <v>1.9848000000000001E-2</v>
-      </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="8"/>
+        <v>8.0254000000000006E-2</v>
+      </c>
+      <c r="E15" s="11"/>
+      <c r="F15" s="14"/>
       <c r="G15" s="3">
-        <v>2.326114</v>
-      </c>
-      <c r="H15" s="5"/>
-      <c r="I15" s="8"/>
+        <v>1.0534650000000001</v>
+      </c>
+      <c r="H15" s="11"/>
+      <c r="I15" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="D3:D7"/>
-    <mergeCell ref="F3:F7"/>
-    <mergeCell ref="A9:I9"/>
     <mergeCell ref="I11:I15"/>
     <mergeCell ref="B11:B15"/>
     <mergeCell ref="C11:C15"/>
     <mergeCell ref="E11:E15"/>
     <mergeCell ref="F11:F15"/>
     <mergeCell ref="H11:H15"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="D3:D7"/>
+    <mergeCell ref="F3:F7"/>
+    <mergeCell ref="A9:I9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1288,7 +1288,7 @@
   <dimension ref="A1:L39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="A9" sqref="A9:L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1303,16 +1303,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -1344,28 +1344,28 @@
       <c r="A3" s="1">
         <v>7.7799999999999996E-3</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="7">
         <f>AVERAGE(A3:A7)</f>
         <v>6.4991999999999992E-3</v>
       </c>
       <c r="C3" s="1">
         <v>3.4301999999999999E-2</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="7">
         <f>AVERAGE(C3:C7)</f>
         <v>4.93788E-2</v>
       </c>
       <c r="E3" s="1">
         <v>2.4107050000000001</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="7">
         <f>AVERAGE(E3:E7)</f>
         <v>2.3921540000000001</v>
       </c>
       <c r="G3" s="1">
         <v>23.769746000000001</v>
       </c>
-      <c r="H3" s="12">
+      <c r="H3" s="7">
         <f>AVERAGE(G3:G7)</f>
         <v>23.8937372</v>
       </c>
@@ -1374,89 +1374,89 @@
       <c r="A4" s="1">
         <v>5.986E-3</v>
       </c>
-      <c r="B4" s="12"/>
+      <c r="B4" s="7"/>
       <c r="C4" s="1">
         <v>3.2233999999999999E-2</v>
       </c>
-      <c r="D4" s="12"/>
+      <c r="D4" s="7"/>
       <c r="E4" s="1">
         <v>2.3849840000000002</v>
       </c>
-      <c r="F4" s="12"/>
+      <c r="F4" s="7"/>
       <c r="G4" s="1">
         <v>23.880281</v>
       </c>
-      <c r="H4" s="12"/>
+      <c r="H4" s="7"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>6.3420000000000004E-3</v>
       </c>
-      <c r="B5" s="12"/>
+      <c r="B5" s="7"/>
       <c r="C5" s="1">
         <v>3.2267999999999998E-2</v>
       </c>
-      <c r="D5" s="12"/>
+      <c r="D5" s="7"/>
       <c r="E5" s="1">
         <v>2.418174</v>
       </c>
-      <c r="F5" s="12"/>
+      <c r="F5" s="7"/>
       <c r="G5" s="1">
         <v>23.901166</v>
       </c>
-      <c r="H5" s="12"/>
+      <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>6.0850000000000001E-3</v>
       </c>
-      <c r="B6" s="12"/>
+      <c r="B6" s="7"/>
       <c r="C6" s="1">
         <v>6.1054999999999998E-2</v>
       </c>
-      <c r="D6" s="12"/>
+      <c r="D6" s="7"/>
       <c r="E6" s="1">
         <v>2.374854</v>
       </c>
-      <c r="F6" s="12"/>
+      <c r="F6" s="7"/>
       <c r="G6" s="1">
         <v>23.998033</v>
       </c>
-      <c r="H6" s="12"/>
+      <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6.3029999999999996E-3</v>
       </c>
-      <c r="B7" s="12"/>
+      <c r="B7" s="7"/>
       <c r="C7" s="1">
         <v>8.7035000000000001E-2</v>
       </c>
-      <c r="D7" s="12"/>
+      <c r="D7" s="7"/>
       <c r="E7" s="1">
         <v>2.3720530000000002</v>
       </c>
-      <c r="F7" s="12"/>
+      <c r="F7" s="7"/>
       <c r="G7" s="1">
         <v>23.919460000000001</v>
       </c>
-      <c r="H7" s="12"/>
+      <c r="H7" s="7"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
@@ -1500,44 +1500,44 @@
       <c r="A11" s="3">
         <v>4.3769999999999998E-3</v>
       </c>
-      <c r="B11" s="22">
+      <c r="B11" s="24">
         <f>AVERAGE(A11:A15)</f>
         <v>4.4596000000000002E-3</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="12">
         <f>B3/B11</f>
         <v>1.4573504350165931</v>
       </c>
       <c r="D11" s="3">
         <v>6.8006999999999998E-2</v>
       </c>
-      <c r="E11" s="22">
+      <c r="E11" s="24">
         <f>AVERAGE(D11:D15)</f>
         <v>6.4985799999999996E-2</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="12">
         <f>D3/E11</f>
         <v>0.75983984193469967</v>
       </c>
       <c r="G11" s="3">
         <v>6.6232480000000002</v>
       </c>
-      <c r="H11" s="22">
+      <c r="H11" s="24">
         <f>AVERAGE(G11:G15)</f>
         <v>6.686429200000001</v>
       </c>
-      <c r="I11" s="6">
+      <c r="I11" s="12">
         <f>F3/H11</f>
         <v>0.3577625558347346</v>
       </c>
       <c r="J11" s="3">
         <v>89.042483000000004</v>
       </c>
-      <c r="K11" s="22">
+      <c r="K11" s="24">
         <f>AVERAGE(J11:J15)</f>
         <v>74.137772400000017</v>
       </c>
-      <c r="L11" s="6">
+      <c r="L11" s="12">
         <f>H3/K11</f>
         <v>0.32228830765354899</v>
       </c>
@@ -1546,105 +1546,105 @@
       <c r="A12" s="3">
         <v>4.4380000000000001E-3</v>
       </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="7"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="13"/>
       <c r="D12" s="3">
         <v>4.1998000000000001E-2</v>
       </c>
-      <c r="E12" s="23"/>
-      <c r="F12" s="7"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="13"/>
       <c r="G12" s="3">
         <v>6.5891760000000001</v>
       </c>
-      <c r="H12" s="23"/>
-      <c r="I12" s="7"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="13"/>
       <c r="J12" s="3">
         <v>71.662083999999993</v>
       </c>
-      <c r="K12" s="23"/>
-      <c r="L12" s="7"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="13"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>4.5110000000000003E-3</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="7"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="13"/>
       <c r="D13" s="3">
         <v>4.3872000000000001E-2</v>
       </c>
-      <c r="E13" s="23"/>
-      <c r="F13" s="7"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="13"/>
       <c r="G13" s="3">
         <v>6.7215730000000002</v>
       </c>
-      <c r="H13" s="23"/>
-      <c r="I13" s="7"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="13"/>
       <c r="J13" s="3">
         <v>69.002851000000007</v>
       </c>
-      <c r="K13" s="23"/>
-      <c r="L13" s="7"/>
+      <c r="K13" s="25"/>
+      <c r="L13" s="13"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>4.5250000000000004E-3</v>
       </c>
-      <c r="B14" s="23"/>
-      <c r="C14" s="7"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="13"/>
       <c r="D14" s="3">
         <v>5.8254E-2</v>
       </c>
-      <c r="E14" s="23"/>
-      <c r="F14" s="7"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="13"/>
       <c r="G14" s="3">
         <v>6.7527499999999998</v>
       </c>
-      <c r="H14" s="23"/>
-      <c r="I14" s="7"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="13"/>
       <c r="J14" s="3">
         <v>68.275855000000007</v>
       </c>
-      <c r="K14" s="23"/>
-      <c r="L14" s="7"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="13"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>4.4470000000000004E-3</v>
       </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="8"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="14"/>
       <c r="D15" s="3">
         <v>0.112798</v>
       </c>
-      <c r="E15" s="24"/>
-      <c r="F15" s="8"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="14"/>
       <c r="G15" s="3">
         <v>6.7453989999999999</v>
       </c>
-      <c r="H15" s="24"/>
-      <c r="I15" s="8"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="14"/>
       <c r="J15" s="3">
         <v>72.705589000000003</v>
       </c>
-      <c r="K15" s="24"/>
-      <c r="L15" s="8"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="14"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
@@ -1688,44 +1688,44 @@
       <c r="A19" s="3">
         <v>4.8999999999999998E-3</v>
       </c>
-      <c r="B19" s="22">
+      <c r="B19" s="24">
         <f>AVERAGE(A19:A23)</f>
         <v>4.6842000000000003E-3</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="12">
         <f>B3/B19</f>
         <v>1.3874727808377094</v>
       </c>
       <c r="D19" s="3">
         <v>5.6577000000000002E-2</v>
       </c>
-      <c r="E19" s="22">
+      <c r="E19" s="24">
         <f>AVERAGE(D19:D23)</f>
         <v>4.8751799999999998E-2</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19" s="12">
         <f>D3/E19</f>
         <v>1.0128610635914983</v>
       </c>
       <c r="G19" s="3">
         <v>3.4884689999999998</v>
       </c>
-      <c r="H19" s="22">
+      <c r="H19" s="24">
         <f>AVERAGE(G19:G23)</f>
         <v>3.6097006</v>
       </c>
-      <c r="I19" s="6">
+      <c r="I19" s="12">
         <f>F3/H19</f>
         <v>0.6627014993985928</v>
       </c>
       <c r="J19" s="3">
         <v>40.36327</v>
       </c>
-      <c r="K19" s="22">
+      <c r="K19" s="24">
         <f>AVERAGE(J19:J23)</f>
         <v>41.001088199999991</v>
       </c>
-      <c r="L19" s="6">
+      <c r="L19" s="12">
         <f>H3/K19</f>
         <v>0.58275861078243296</v>
       </c>
@@ -1734,105 +1734,105 @@
       <c r="A20" s="3">
         <v>4.7720000000000002E-3</v>
       </c>
-      <c r="B20" s="23"/>
-      <c r="C20" s="7"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="13"/>
       <c r="D20" s="3">
         <v>6.0916999999999999E-2</v>
       </c>
-      <c r="E20" s="23"/>
-      <c r="F20" s="7"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="13"/>
       <c r="G20" s="3">
         <v>3.561401</v>
       </c>
-      <c r="H20" s="23"/>
-      <c r="I20" s="7"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="13"/>
       <c r="J20" s="3">
         <v>47.20411</v>
       </c>
-      <c r="K20" s="23"/>
-      <c r="L20" s="7"/>
+      <c r="K20" s="25"/>
+      <c r="L20" s="13"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>4.9020000000000001E-3</v>
       </c>
-      <c r="B21" s="23"/>
-      <c r="C21" s="7"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="13"/>
       <c r="D21" s="3">
         <v>4.2832000000000002E-2</v>
       </c>
-      <c r="E21" s="23"/>
-      <c r="F21" s="7"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="13"/>
       <c r="G21" s="3">
         <v>3.6326170000000002</v>
       </c>
-      <c r="H21" s="23"/>
-      <c r="I21" s="7"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="13"/>
       <c r="J21" s="3">
         <v>41.847327999999997</v>
       </c>
-      <c r="K21" s="23"/>
-      <c r="L21" s="7"/>
+      <c r="K21" s="25"/>
+      <c r="L21" s="13"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>4.4450000000000002E-3</v>
       </c>
-      <c r="B22" s="23"/>
-      <c r="C22" s="7"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="13"/>
       <c r="D22" s="3">
         <v>4.1216999999999997E-2</v>
       </c>
-      <c r="E22" s="23"/>
-      <c r="F22" s="7"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="13"/>
       <c r="G22" s="3">
         <v>3.6529639999999999</v>
       </c>
-      <c r="H22" s="23"/>
-      <c r="I22" s="7"/>
+      <c r="H22" s="25"/>
+      <c r="I22" s="13"/>
       <c r="J22" s="3">
         <v>37.903092999999998</v>
       </c>
-      <c r="K22" s="23"/>
-      <c r="L22" s="7"/>
+      <c r="K22" s="25"/>
+      <c r="L22" s="13"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>4.4019999999999997E-3</v>
       </c>
-      <c r="B23" s="24"/>
-      <c r="C23" s="8"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="14"/>
       <c r="D23" s="3">
         <v>4.2215999999999997E-2</v>
       </c>
-      <c r="E23" s="24"/>
-      <c r="F23" s="8"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="14"/>
       <c r="G23" s="3">
         <v>3.7130519999999998</v>
       </c>
-      <c r="H23" s="24"/>
-      <c r="I23" s="8"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="14"/>
       <c r="J23" s="3">
         <v>37.687640000000002</v>
       </c>
-      <c r="K23" s="24"/>
-      <c r="L23" s="8"/>
+      <c r="K23" s="26"/>
+      <c r="L23" s="14"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
-      <c r="L25" s="10"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
@@ -1876,44 +1876,44 @@
       <c r="A27" s="3">
         <v>4.3699999999999998E-3</v>
       </c>
-      <c r="B27" s="22">
+      <c r="B27" s="24">
         <f>AVERAGE(A27:A31)</f>
         <v>4.3296000000000003E-3</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C27" s="12">
         <f>B3/B27</f>
         <v>1.5011086474501105</v>
       </c>
       <c r="D27" s="3">
         <v>6.8677000000000002E-2</v>
       </c>
-      <c r="E27" s="22">
+      <c r="E27" s="24">
         <f>AVERAGE(D27:D31)</f>
         <v>5.2304200000000002E-2</v>
       </c>
-      <c r="F27" s="6">
+      <c r="F27" s="12">
         <f>D3/E27</f>
         <v>0.94406950111080945</v>
       </c>
       <c r="G27" s="3">
         <v>1.9634100000000001</v>
       </c>
-      <c r="H27" s="22">
+      <c r="H27" s="24">
         <f>AVERAGE(G27:G31)</f>
         <v>2.189451</v>
       </c>
-      <c r="I27" s="6">
+      <c r="I27" s="12">
         <f>F3/H27</f>
         <v>1.0925816563147566</v>
       </c>
       <c r="J27" s="3">
         <v>22.983543000000001</v>
       </c>
-      <c r="K27" s="22">
+      <c r="K27" s="24">
         <f>AVERAGE(J27:J31)</f>
         <v>24.474444599999998</v>
       </c>
-      <c r="L27" s="6">
+      <c r="L27" s="12">
         <f>H3/K27</f>
         <v>0.97627290794578447</v>
       </c>
@@ -1922,105 +1922,105 @@
       <c r="A28" s="3">
         <v>4.2700000000000004E-3</v>
       </c>
-      <c r="B28" s="23"/>
-      <c r="C28" s="7"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="13"/>
       <c r="D28" s="3">
         <v>4.2324000000000001E-2</v>
       </c>
-      <c r="E28" s="23"/>
-      <c r="F28" s="7"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="13"/>
       <c r="G28" s="3">
         <v>2.1728649999999998</v>
       </c>
-      <c r="H28" s="23"/>
-      <c r="I28" s="7"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="13"/>
       <c r="J28" s="3">
         <v>23.784718999999999</v>
       </c>
-      <c r="K28" s="23"/>
-      <c r="L28" s="7"/>
+      <c r="K28" s="25"/>
+      <c r="L28" s="13"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>4.4650000000000002E-3</v>
       </c>
-      <c r="B29" s="23"/>
-      <c r="C29" s="7"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="13"/>
       <c r="D29" s="3">
         <v>4.3873000000000002E-2</v>
       </c>
-      <c r="E29" s="23"/>
-      <c r="F29" s="7"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="13"/>
       <c r="G29" s="3">
         <v>2.1944849999999998</v>
       </c>
-      <c r="H29" s="23"/>
-      <c r="I29" s="7"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="13"/>
       <c r="J29" s="3">
         <v>25.523700000000002</v>
       </c>
-      <c r="K29" s="23"/>
-      <c r="L29" s="7"/>
+      <c r="K29" s="25"/>
+      <c r="L29" s="13"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>4.3579999999999999E-3</v>
       </c>
-      <c r="B30" s="23"/>
-      <c r="C30" s="7"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="13"/>
       <c r="D30" s="3">
         <v>4.1213E-2</v>
       </c>
-      <c r="E30" s="23"/>
-      <c r="F30" s="7"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="13"/>
       <c r="G30" s="3">
         <v>2.3042750000000001</v>
       </c>
-      <c r="H30" s="23"/>
-      <c r="I30" s="7"/>
+      <c r="H30" s="25"/>
+      <c r="I30" s="13"/>
       <c r="J30" s="3">
         <v>27.042113000000001</v>
       </c>
-      <c r="K30" s="23"/>
-      <c r="L30" s="7"/>
+      <c r="K30" s="25"/>
+      <c r="L30" s="13"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>4.1850000000000004E-3</v>
       </c>
-      <c r="B31" s="24"/>
-      <c r="C31" s="8"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="14"/>
       <c r="D31" s="3">
         <v>6.5434000000000006E-2</v>
       </c>
-      <c r="E31" s="24"/>
-      <c r="F31" s="8"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="14"/>
       <c r="G31" s="3">
         <v>2.3122199999999999</v>
       </c>
-      <c r="H31" s="24"/>
-      <c r="I31" s="8"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="14"/>
       <c r="J31" s="3">
         <v>23.038148</v>
       </c>
-      <c r="K31" s="24"/>
-      <c r="L31" s="8"/>
+      <c r="K31" s="26"/>
+      <c r="L31" s="14"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A33" s="10" t="s">
+      <c r="A33" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="10"/>
-      <c r="I33" s="10"/>
-      <c r="J33" s="10"/>
-      <c r="K33" s="10"/>
-      <c r="L33" s="10"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
@@ -2064,44 +2064,44 @@
       <c r="A35" s="3">
         <v>4.5999999999999999E-3</v>
       </c>
-      <c r="B35" s="22">
+      <c r="B35" s="24">
         <f>AVERAGE(A35:A39)</f>
         <v>5.8130000000000005E-3</v>
       </c>
-      <c r="C35" s="6">
+      <c r="C35" s="12">
         <f>B3/B35</f>
         <v>1.1180457595045585</v>
       </c>
       <c r="D35" s="3">
         <v>4.335E-2</v>
       </c>
-      <c r="E35" s="22">
+      <c r="E35" s="24">
         <f>AVERAGE(D35:D39)</f>
         <v>4.2192600000000004E-2</v>
       </c>
-      <c r="F35" s="6">
+      <c r="F35" s="12">
         <f>D3/E35</f>
         <v>1.1703189658850128</v>
       </c>
       <c r="G35" s="3">
         <v>1.668833</v>
       </c>
-      <c r="H35" s="22">
+      <c r="H35" s="24">
         <f>AVERAGE(G35:G39)</f>
         <v>1.9743895999999999</v>
       </c>
-      <c r="I35" s="6">
+      <c r="I35" s="12">
         <f>F3/H35</f>
         <v>1.2115916737000643</v>
       </c>
       <c r="J35" s="3">
         <v>21.320739</v>
       </c>
-      <c r="K35" s="22">
+      <c r="K35" s="24">
         <f>AVERAGE(J35:J39)</f>
         <v>21.781726599999999</v>
       </c>
-      <c r="L35" s="6">
+      <c r="L35" s="12">
         <f>H3/K35</f>
         <v>1.0969624969950731</v>
       </c>
@@ -2110,98 +2110,111 @@
       <c r="A36" s="3">
         <v>4.5840000000000004E-3</v>
       </c>
-      <c r="B36" s="23"/>
-      <c r="C36" s="7"/>
+      <c r="B36" s="25"/>
+      <c r="C36" s="13"/>
       <c r="D36" s="3">
         <v>4.1674000000000003E-2</v>
       </c>
-      <c r="E36" s="23"/>
-      <c r="F36" s="7"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="13"/>
       <c r="G36" s="3">
         <v>2.009665</v>
       </c>
-      <c r="H36" s="23"/>
-      <c r="I36" s="7"/>
+      <c r="H36" s="25"/>
+      <c r="I36" s="13"/>
       <c r="J36" s="3">
         <v>21.419577</v>
       </c>
-      <c r="K36" s="23"/>
-      <c r="L36" s="7"/>
+      <c r="K36" s="25"/>
+      <c r="L36" s="13"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>7.3130000000000001E-3</v>
       </c>
-      <c r="B37" s="23"/>
-      <c r="C37" s="7"/>
+      <c r="B37" s="25"/>
+      <c r="C37" s="13"/>
       <c r="D37" s="3">
         <v>4.2286999999999998E-2</v>
       </c>
-      <c r="E37" s="23"/>
-      <c r="F37" s="7"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="13"/>
       <c r="G37" s="3">
         <v>2.188358</v>
       </c>
-      <c r="H37" s="23"/>
-      <c r="I37" s="7"/>
+      <c r="H37" s="25"/>
+      <c r="I37" s="13"/>
       <c r="J37" s="3">
         <v>21.917483000000001</v>
       </c>
-      <c r="K37" s="23"/>
-      <c r="L37" s="7"/>
+      <c r="K37" s="25"/>
+      <c r="L37" s="13"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>4.6990000000000001E-3</v>
       </c>
-      <c r="B38" s="23"/>
-      <c r="C38" s="7"/>
+      <c r="B38" s="25"/>
+      <c r="C38" s="13"/>
       <c r="D38" s="3">
         <v>4.1896999999999997E-2</v>
       </c>
-      <c r="E38" s="23"/>
-      <c r="F38" s="7"/>
+      <c r="E38" s="25"/>
+      <c r="F38" s="13"/>
       <c r="G38" s="3">
         <v>2.0170970000000001</v>
       </c>
-      <c r="H38" s="23"/>
-      <c r="I38" s="7"/>
+      <c r="H38" s="25"/>
+      <c r="I38" s="13"/>
       <c r="J38" s="3">
         <v>22.68177</v>
       </c>
-      <c r="K38" s="23"/>
-      <c r="L38" s="7"/>
+      <c r="K38" s="25"/>
+      <c r="L38" s="13"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>7.8689999999999993E-3</v>
       </c>
-      <c r="B39" s="24"/>
-      <c r="C39" s="8"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="14"/>
       <c r="D39" s="3">
         <v>4.1755E-2</v>
       </c>
-      <c r="E39" s="24"/>
-      <c r="F39" s="8"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="14"/>
       <c r="G39" s="3">
         <v>1.987995</v>
       </c>
-      <c r="H39" s="24"/>
-      <c r="I39" s="8"/>
+      <c r="H39" s="26"/>
+      <c r="I39" s="14"/>
       <c r="J39" s="3">
         <v>21.569064000000001</v>
       </c>
-      <c r="K39" s="24"/>
-      <c r="L39" s="8"/>
+      <c r="K39" s="26"/>
+      <c r="L39" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="A9:L9"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="D3:D7"/>
-    <mergeCell ref="F3:F7"/>
-    <mergeCell ref="H3:H7"/>
+    <mergeCell ref="A33:L33"/>
+    <mergeCell ref="B35:B39"/>
+    <mergeCell ref="C35:C39"/>
+    <mergeCell ref="E35:E39"/>
+    <mergeCell ref="F35:F39"/>
+    <mergeCell ref="H35:H39"/>
+    <mergeCell ref="I35:I39"/>
+    <mergeCell ref="K35:K39"/>
+    <mergeCell ref="L35:L39"/>
+    <mergeCell ref="L19:L23"/>
+    <mergeCell ref="A25:L25"/>
+    <mergeCell ref="B27:B31"/>
+    <mergeCell ref="C27:C31"/>
+    <mergeCell ref="E27:E31"/>
+    <mergeCell ref="F27:F31"/>
+    <mergeCell ref="H27:H31"/>
+    <mergeCell ref="I27:I31"/>
+    <mergeCell ref="K27:K31"/>
+    <mergeCell ref="L27:L31"/>
     <mergeCell ref="K11:K15"/>
     <mergeCell ref="L11:L15"/>
     <mergeCell ref="A17:L17"/>
@@ -2218,25 +2231,12 @@
     <mergeCell ref="F11:F15"/>
     <mergeCell ref="H11:H15"/>
     <mergeCell ref="I11:I15"/>
-    <mergeCell ref="L19:L23"/>
-    <mergeCell ref="A25:L25"/>
-    <mergeCell ref="B27:B31"/>
-    <mergeCell ref="C27:C31"/>
-    <mergeCell ref="E27:E31"/>
-    <mergeCell ref="F27:F31"/>
-    <mergeCell ref="H27:H31"/>
-    <mergeCell ref="I27:I31"/>
-    <mergeCell ref="K27:K31"/>
-    <mergeCell ref="L27:L31"/>
-    <mergeCell ref="A33:L33"/>
-    <mergeCell ref="B35:B39"/>
-    <mergeCell ref="C35:C39"/>
-    <mergeCell ref="E35:E39"/>
-    <mergeCell ref="F35:F39"/>
-    <mergeCell ref="H35:H39"/>
-    <mergeCell ref="I35:I39"/>
-    <mergeCell ref="K35:K39"/>
-    <mergeCell ref="L35:L39"/>
+    <mergeCell ref="A9:L9"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="D3:D7"/>
+    <mergeCell ref="F3:F7"/>
+    <mergeCell ref="H3:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Corrected times for MPI programs.
Added -O3 flag for compiler optimizations when compiling.
</commit_message>
<xml_diff>
--- a/CUDA/racunanje_ubrzanja_programa_cuda.xlsx
+++ b/CUDA/racunanje_ubrzanja_programa_cuda.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saren\OneDrive\Documents\ETF\7. semestar\Multiprocesorski sistemi\GitHub_Domaci\Multiprocessing_Systems\CUDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C969194B-B5EE-4145-A427-CC97F84109FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2B8122-671E-4E45-BB42-CB9F446D6823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{E700D36A-9AEC-48B1-B431-3A7C21838328}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E700D36A-9AEC-48B1-B431-3A7C21838328}"/>
   </bookViews>
   <sheets>
     <sheet name="Zadatak 1" sheetId="3" r:id="rId1"/>
@@ -646,8 +646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E507908-E47E-43FA-866F-ABBDC664C0C3}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -692,49 +692,49 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>4.0029999999999996E-3</v>
+        <v>9.9299999999999996E-4</v>
       </c>
       <c r="B3" s="7">
         <f>AVERAGE(A3:A7)</f>
-        <v>3.9849999999999998E-3</v>
+        <v>3.1570000000000001E-3</v>
       </c>
       <c r="C3" s="1">
-        <v>1.0662E-2</v>
+        <v>8.6459999999999992E-3</v>
       </c>
       <c r="D3" s="7">
         <f>AVERAGE(C3:C7)</f>
-        <v>1.0530999999999999E-2</v>
+        <v>9.7502000000000005E-3</v>
       </c>
       <c r="E3" s="1">
-        <v>0.22844900000000001</v>
+        <v>0.17707700000000001</v>
       </c>
       <c r="F3" s="7">
         <f>AVERAGE(E3:E7)</f>
-        <v>0.21360760000000001</v>
+        <v>0.19951760000000002</v>
       </c>
       <c r="G3" s="1">
-        <v>4.5852110000000001</v>
+        <v>4.2143699999999997</v>
       </c>
       <c r="H3" s="8">
         <f>AVERAGE(G3:G7)</f>
-        <v>4.6139513999999995</v>
+        <v>4.4418106000000002</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>3.9899999999999996E-3</v>
+        <v>2.8600000000000001E-3</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="1">
-        <v>1.0253999999999999E-2</v>
+        <v>8.3660000000000002E-3</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="1">
-        <v>0.19584399999999999</v>
+        <v>0.17676600000000001</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="1">
-        <v>4.7025360000000003</v>
+        <v>4.2126729999999997</v>
       </c>
       <c r="H4" s="9"/>
     </row>
@@ -856,7 +856,7 @@
       </c>
       <c r="C11" s="15">
         <f>B3/B11</f>
-        <v>14.629221732745961</v>
+        <v>11.58957415565345</v>
       </c>
       <c r="D11" s="3">
         <v>4.4000000000000002E-4</v>
@@ -867,7 +867,7 @@
       </c>
       <c r="F11" s="12">
         <f>D3/E11</f>
-        <v>23.955868971792533</v>
+        <v>22.179708826205641</v>
       </c>
       <c r="G11" s="3">
         <v>3.333E-3</v>
@@ -878,7 +878,7 @@
       </c>
       <c r="I11" s="12">
         <f>F3/H11</f>
-        <v>64.069466106778648</v>
+        <v>59.843311337732459</v>
       </c>
       <c r="J11" s="3">
         <v>8.0574999999999994E-2</v>
@@ -889,7 +889,7 @@
       </c>
       <c r="L11" s="12">
         <f>H3/K11</f>
-        <v>57.273335964905741</v>
+        <v>55.136538886447653</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
@@ -1005,7 +1005,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7851D13-C089-4E79-B982-DBF5982D0E6F}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
First try of dz4z3.cu.
Doesn't have correct results.
</commit_message>
<xml_diff>
--- a/CUDA/racunanje_ubrzanja_programa_cuda.xlsx
+++ b/CUDA/racunanje_ubrzanja_programa_cuda.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saren\OneDrive\Documents\ETF\7. semestar\Multiprocesorski sistemi\GitHub_Domaci\Multiprocessing_Systems\CUDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2B8122-671E-4E45-BB42-CB9F446D6823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36BEA473-BC68-402A-82BE-1C09328C4E2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E700D36A-9AEC-48B1-B431-3A7C21838328}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{E700D36A-9AEC-48B1-B431-3A7C21838328}"/>
   </bookViews>
   <sheets>
     <sheet name="Zadatak 1" sheetId="3" r:id="rId1"/>
@@ -264,6 +264,21 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -282,21 +297,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -315,20 +315,20 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -646,23 +646,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E507908-E47E-43FA-866F-ABBDC664C0C3}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
@@ -692,121 +692,121 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>9.9299999999999996E-4</v>
-      </c>
-      <c r="B3" s="7">
+        <v>2.859E-3</v>
+      </c>
+      <c r="B3" s="12">
         <f>AVERAGE(A3:A7)</f>
-        <v>3.1570000000000001E-3</v>
+        <v>2.8677999999999998E-3</v>
       </c>
       <c r="C3" s="1">
-        <v>8.6459999999999992E-3</v>
-      </c>
-      <c r="D3" s="7">
+        <v>9.2750000000000003E-3</v>
+      </c>
+      <c r="D3" s="12">
         <f>AVERAGE(C3:C7)</f>
-        <v>9.7502000000000005E-3</v>
+        <v>9.2186000000000021E-3</v>
       </c>
       <c r="E3" s="1">
-        <v>0.17707700000000001</v>
-      </c>
-      <c r="F3" s="7">
+        <v>0.176201</v>
+      </c>
+      <c r="F3" s="12">
         <f>AVERAGE(E3:E7)</f>
-        <v>0.19951760000000002</v>
+        <v>0.17561979999999999</v>
       </c>
       <c r="G3" s="1">
-        <v>4.2143699999999997</v>
-      </c>
-      <c r="H3" s="8">
+        <v>4.1992710000000004</v>
+      </c>
+      <c r="H3" s="13">
         <f>AVERAGE(G3:G7)</f>
-        <v>4.4418106000000002</v>
+        <v>4.1829993999999999</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>2.8600000000000001E-3</v>
-      </c>
-      <c r="B4" s="7"/>
+        <v>2.872E-3</v>
+      </c>
+      <c r="B4" s="12"/>
       <c r="C4" s="1">
-        <v>8.3660000000000002E-3</v>
-      </c>
-      <c r="D4" s="7"/>
+        <v>1.0198E-2</v>
+      </c>
+      <c r="D4" s="12"/>
       <c r="E4" s="1">
-        <v>0.17676600000000001</v>
-      </c>
-      <c r="F4" s="7"/>
+        <v>0.176263</v>
+      </c>
+      <c r="F4" s="12"/>
       <c r="G4" s="1">
-        <v>4.2126729999999997</v>
-      </c>
-      <c r="H4" s="9"/>
+        <v>4.2012299999999998</v>
+      </c>
+      <c r="H4" s="14"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>4.1009999999999996E-3</v>
-      </c>
-      <c r="B5" s="7"/>
+        <v>2.8570000000000002E-3</v>
+      </c>
+      <c r="B5" s="12"/>
       <c r="C5" s="1">
-        <v>1.0397999999999999E-2</v>
-      </c>
-      <c r="D5" s="7"/>
+        <v>9.7560000000000008E-3</v>
+      </c>
+      <c r="D5" s="12"/>
       <c r="E5" s="1">
-        <v>0.20313800000000001</v>
-      </c>
-      <c r="F5" s="7"/>
+        <v>0.17635200000000001</v>
+      </c>
+      <c r="F5" s="12"/>
       <c r="G5" s="1">
-        <v>4.608962</v>
-      </c>
-      <c r="H5" s="9"/>
+        <v>4.1154200000000003</v>
+      </c>
+      <c r="H5" s="14"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>3.9529999999999999E-3</v>
-      </c>
-      <c r="B6" s="7"/>
+        <v>2.9009999999999999E-3</v>
+      </c>
+      <c r="B6" s="12"/>
       <c r="C6" s="1">
-        <v>1.0951000000000001E-2</v>
-      </c>
-      <c r="D6" s="7"/>
+        <v>8.5199999999999998E-3</v>
+      </c>
+      <c r="D6" s="12"/>
       <c r="E6" s="1">
-        <v>0.19843</v>
-      </c>
-      <c r="F6" s="7"/>
+        <v>0.17640700000000001</v>
+      </c>
+      <c r="F6" s="12"/>
       <c r="G6" s="1">
-        <v>4.6466500000000002</v>
-      </c>
-      <c r="H6" s="9"/>
+        <v>4.1990109999999996</v>
+      </c>
+      <c r="H6" s="14"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>3.8779999999999999E-3</v>
-      </c>
-      <c r="B7" s="7"/>
+        <v>2.8500000000000001E-3</v>
+      </c>
+      <c r="B7" s="12"/>
       <c r="C7" s="1">
-        <v>1.039E-2</v>
-      </c>
-      <c r="D7" s="7"/>
+        <v>8.3440000000000007E-3</v>
+      </c>
+      <c r="D7" s="12"/>
       <c r="E7" s="1">
-        <v>0.242177</v>
-      </c>
-      <c r="F7" s="7"/>
+        <v>0.172876</v>
+      </c>
+      <c r="F7" s="12"/>
       <c r="G7" s="1">
-        <v>4.5263980000000004</v>
-      </c>
-      <c r="H7" s="10"/>
+        <v>4.2000650000000004</v>
+      </c>
+      <c r="H7" s="15"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
@@ -850,138 +850,144 @@
       <c r="A11" s="3">
         <v>2.7099999999999997E-4</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="5">
         <f>AVERAGE(A11:A15)</f>
         <v>2.7240000000000001E-4</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="9">
         <f>B3/B11</f>
-        <v>11.58957415565345</v>
+        <v>10.527900146842876</v>
       </c>
       <c r="D11" s="3">
         <v>4.4000000000000002E-4</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="5">
         <f>AVERAGE(D11:D15)</f>
         <v>4.3960000000000006E-4</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="6">
         <f>D3/E11</f>
-        <v>22.179708826205641</v>
+        <v>20.970427661510467</v>
       </c>
       <c r="G11" s="3">
         <v>3.333E-3</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="5">
         <f>AVERAGE(G11:G15)</f>
         <v>3.3340000000000002E-3</v>
       </c>
-      <c r="I11" s="12">
+      <c r="I11" s="6">
         <f>F3/H11</f>
-        <v>59.843311337732459</v>
+        <v>52.675404919016195</v>
       </c>
       <c r="J11" s="3">
         <v>8.0574999999999994E-2</v>
       </c>
-      <c r="K11" s="11">
+      <c r="K11" s="5">
         <f>AVERAGE(J11:J15)</f>
         <v>8.0560199999999998E-2</v>
       </c>
-      <c r="L11" s="12">
+      <c r="L11" s="6">
         <f>H3/K11</f>
-        <v>55.136538886447653</v>
+        <v>51.923895422305307</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>2.63E-4</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="15"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="9"/>
       <c r="D12" s="3">
         <v>4.3899999999999999E-4</v>
       </c>
-      <c r="E12" s="11"/>
-      <c r="F12" s="13"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="7"/>
       <c r="G12" s="3">
         <v>3.3249999999999998E-3</v>
       </c>
-      <c r="H12" s="11"/>
-      <c r="I12" s="13"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="7"/>
       <c r="J12" s="3">
         <v>8.0686999999999995E-2</v>
       </c>
-      <c r="K12" s="11"/>
-      <c r="L12" s="13"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="7"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>2.7599999999999999E-4</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="15"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="9"/>
       <c r="D13" s="3">
         <v>4.4099999999999999E-4</v>
       </c>
-      <c r="E13" s="11"/>
-      <c r="F13" s="13"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="7"/>
       <c r="G13" s="3">
         <v>3.3349999999999999E-3</v>
       </c>
-      <c r="H13" s="11"/>
-      <c r="I13" s="13"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="7"/>
       <c r="J13" s="3">
         <v>8.0436999999999995E-2</v>
       </c>
-      <c r="K13" s="11"/>
-      <c r="L13" s="13"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="7"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>2.7700000000000001E-4</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="15"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="9"/>
       <c r="D14" s="3">
         <v>4.4200000000000001E-4</v>
       </c>
-      <c r="E14" s="11"/>
-      <c r="F14" s="13"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="7"/>
       <c r="G14" s="3">
         <v>3.339E-3</v>
       </c>
-      <c r="H14" s="11"/>
-      <c r="I14" s="13"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="7"/>
       <c r="J14" s="3">
         <v>8.0562999999999996E-2</v>
       </c>
-      <c r="K14" s="11"/>
-      <c r="L14" s="13"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="7"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>2.7500000000000002E-4</v>
       </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="15"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="9"/>
       <c r="D15" s="3">
         <v>4.3600000000000003E-4</v>
       </c>
-      <c r="E15" s="11"/>
-      <c r="F15" s="14"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="8"/>
       <c r="G15" s="3">
         <v>3.3379999999999998E-3</v>
       </c>
-      <c r="H15" s="11"/>
-      <c r="I15" s="14"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="8"/>
       <c r="J15" s="3">
         <v>8.0538999999999999E-2</v>
       </c>
-      <c r="K15" s="11"/>
-      <c r="L15" s="14"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A9:L9"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="D3:D7"/>
+    <mergeCell ref="F3:F7"/>
+    <mergeCell ref="H3:H7"/>
     <mergeCell ref="K11:K15"/>
     <mergeCell ref="L11:L15"/>
     <mergeCell ref="B11:B15"/>
@@ -990,12 +996,6 @@
     <mergeCell ref="F11:F15"/>
     <mergeCell ref="H11:H15"/>
     <mergeCell ref="I11:I15"/>
-    <mergeCell ref="A9:L9"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="D3:D7"/>
-    <mergeCell ref="F3:F7"/>
-    <mergeCell ref="H3:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1005,8 +1005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7851D13-C089-4E79-B982-DBF5982D0E6F}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1043,82 +1043,82 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>4.241E-3</v>
-      </c>
-      <c r="B3" s="7">
+        <v>1.438E-3</v>
+      </c>
+      <c r="B3" s="12">
         <f>AVERAGE(A3:A7)</f>
-        <v>2.1372000000000001E-3</v>
+        <v>1.9784000000000004E-3</v>
       </c>
       <c r="C3" s="1">
-        <v>2.8559000000000001E-2</v>
-      </c>
-      <c r="D3" s="7">
+        <v>2.1944000000000002E-2</v>
+      </c>
+      <c r="D3" s="12">
         <f>AVERAGE(C3:C7)</f>
-        <v>2.7738400000000003E-2</v>
+        <v>2.25554E-2</v>
       </c>
       <c r="E3" s="1">
-        <v>2.2680989999999999</v>
-      </c>
-      <c r="F3" s="7">
+        <v>2.4267289999999999</v>
+      </c>
+      <c r="F3" s="12">
         <f>AVERAGE(E3:E7)</f>
-        <v>2.2161198</v>
+        <v>2.2378609999999997</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>1.5939999999999999E-3</v>
-      </c>
-      <c r="B4" s="7"/>
+        <v>1.317E-3</v>
+      </c>
+      <c r="B4" s="12"/>
       <c r="C4" s="1">
-        <v>2.7979E-2</v>
-      </c>
-      <c r="D4" s="7"/>
+        <v>2.9302000000000002E-2</v>
+      </c>
+      <c r="D4" s="12"/>
       <c r="E4" s="1">
-        <v>2.19848</v>
-      </c>
-      <c r="F4" s="7"/>
+        <v>1.8761060000000001</v>
+      </c>
+      <c r="F4" s="12"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>1.56E-3</v>
-      </c>
-      <c r="B5" s="7"/>
+        <v>3.32E-3</v>
+      </c>
+      <c r="B5" s="12"/>
       <c r="C5" s="1">
-        <v>2.3862999999999999E-2</v>
-      </c>
-      <c r="D5" s="7"/>
+        <v>2.3130000000000001E-2</v>
+      </c>
+      <c r="D5" s="12"/>
       <c r="E5" s="1">
-        <v>2.2217060000000002</v>
-      </c>
-      <c r="F5" s="7"/>
+        <v>2.4563670000000002</v>
+      </c>
+      <c r="F5" s="12"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>1.663E-3</v>
-      </c>
-      <c r="B6" s="7"/>
+        <v>1.47E-3</v>
+      </c>
+      <c r="B6" s="12"/>
       <c r="C6" s="1">
-        <v>3.1158000000000002E-2</v>
-      </c>
-      <c r="D6" s="7"/>
+        <v>1.6910000000000001E-2</v>
+      </c>
+      <c r="D6" s="12"/>
       <c r="E6" s="1">
-        <v>2.086471</v>
-      </c>
-      <c r="F6" s="7"/>
+        <v>2.0546519999999999</v>
+      </c>
+      <c r="F6" s="12"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>1.6280000000000001E-3</v>
-      </c>
-      <c r="B7" s="7"/>
+        <v>2.3470000000000001E-3</v>
+      </c>
+      <c r="B7" s="12"/>
       <c r="C7" s="1">
-        <v>2.7133000000000001E-2</v>
-      </c>
-      <c r="D7" s="7"/>
+        <v>2.1491E-2</v>
+      </c>
+      <c r="D7" s="12"/>
       <c r="E7" s="1">
-        <v>2.3058429999999999</v>
-      </c>
-      <c r="F7" s="7"/>
+        <v>2.375451</v>
+      </c>
+      <c r="F7" s="12"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="19" t="s">
@@ -1166,118 +1166,118 @@
       <c r="A11" s="3">
         <v>9.5614000000000005E-2</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="5">
         <f>AVERAGE(A11:A15)</f>
         <v>8.6125800000000002E-2</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="9">
         <f>B3/B11</f>
-        <v>2.4814863838710351E-2</v>
+        <v>2.2971049325521509E-2</v>
       </c>
       <c r="D11" s="3">
         <v>8.5962999999999998E-2</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="5">
         <f>AVERAGE(D11:D15)</f>
         <v>8.4431400000000004E-2</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="6">
         <f>D3/E11</f>
-        <v>0.32853180214943734</v>
+        <v>0.26714468787678514</v>
       </c>
       <c r="G11" s="3">
         <v>1.0524530000000001</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="5">
         <f>AVERAGE(G11:G15)</f>
         <v>1.0546840000000002</v>
       </c>
-      <c r="I11" s="12">
+      <c r="I11" s="6">
         <f>F3/H11</f>
-        <v>2.1012168573714969</v>
+        <v>2.1218308042977796</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>9.0286000000000005E-2</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="15"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="9"/>
       <c r="D12" s="3">
         <v>9.2688000000000006E-2</v>
       </c>
-      <c r="E12" s="11"/>
-      <c r="F12" s="13"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="7"/>
       <c r="G12" s="3">
         <v>1.049847</v>
       </c>
-      <c r="H12" s="11"/>
-      <c r="I12" s="13"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="7"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>9.1924000000000006E-2</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="15"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="9"/>
       <c r="D13" s="3">
         <v>8.2306000000000004E-2</v>
       </c>
-      <c r="E13" s="11"/>
-      <c r="F13" s="13"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="7"/>
       <c r="G13" s="3">
         <v>1.0593520000000001</v>
       </c>
-      <c r="H13" s="11"/>
-      <c r="I13" s="13"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="7"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>8.3705000000000002E-2</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="15"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="9"/>
       <c r="D14" s="3">
         <v>8.0946000000000004E-2</v>
       </c>
-      <c r="E14" s="11"/>
-      <c r="F14" s="13"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="7"/>
       <c r="G14" s="3">
         <v>1.058303</v>
       </c>
-      <c r="H14" s="11"/>
-      <c r="I14" s="13"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="7"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>6.9099999999999995E-2</v>
       </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="15"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="9"/>
       <c r="D15" s="3">
         <v>8.0254000000000006E-2</v>
       </c>
-      <c r="E15" s="11"/>
-      <c r="F15" s="14"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="8"/>
       <c r="G15" s="3">
         <v>1.0534650000000001</v>
       </c>
-      <c r="H15" s="11"/>
-      <c r="I15" s="14"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="D3:D7"/>
+    <mergeCell ref="F3:F7"/>
+    <mergeCell ref="A9:I9"/>
     <mergeCell ref="I11:I15"/>
     <mergeCell ref="B11:B15"/>
     <mergeCell ref="C11:C15"/>
     <mergeCell ref="E11:E15"/>
     <mergeCell ref="F11:F15"/>
     <mergeCell ref="H11:H15"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="D3:D7"/>
-    <mergeCell ref="F3:F7"/>
-    <mergeCell ref="A9:I9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1303,16 +1303,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -1344,28 +1344,28 @@
       <c r="A3" s="1">
         <v>7.7799999999999996E-3</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="12">
         <f>AVERAGE(A3:A7)</f>
         <v>6.4991999999999992E-3</v>
       </c>
       <c r="C3" s="1">
         <v>3.4301999999999999E-2</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="12">
         <f>AVERAGE(C3:C7)</f>
         <v>4.93788E-2</v>
       </c>
       <c r="E3" s="1">
         <v>2.4107050000000001</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="12">
         <f>AVERAGE(E3:E7)</f>
         <v>2.3921540000000001</v>
       </c>
       <c r="G3" s="1">
         <v>23.769746000000001</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="12">
         <f>AVERAGE(G3:G7)</f>
         <v>23.8937372</v>
       </c>
@@ -1374,89 +1374,89 @@
       <c r="A4" s="1">
         <v>5.986E-3</v>
       </c>
-      <c r="B4" s="7"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="1">
         <v>3.2233999999999999E-2</v>
       </c>
-      <c r="D4" s="7"/>
+      <c r="D4" s="12"/>
       <c r="E4" s="1">
         <v>2.3849840000000002</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="F4" s="12"/>
       <c r="G4" s="1">
         <v>23.880281</v>
       </c>
-      <c r="H4" s="7"/>
+      <c r="H4" s="12"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>6.3420000000000004E-3</v>
       </c>
-      <c r="B5" s="7"/>
+      <c r="B5" s="12"/>
       <c r="C5" s="1">
         <v>3.2267999999999998E-2</v>
       </c>
-      <c r="D5" s="7"/>
+      <c r="D5" s="12"/>
       <c r="E5" s="1">
         <v>2.418174</v>
       </c>
-      <c r="F5" s="7"/>
+      <c r="F5" s="12"/>
       <c r="G5" s="1">
         <v>23.901166</v>
       </c>
-      <c r="H5" s="7"/>
+      <c r="H5" s="12"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>6.0850000000000001E-3</v>
       </c>
-      <c r="B6" s="7"/>
+      <c r="B6" s="12"/>
       <c r="C6" s="1">
         <v>6.1054999999999998E-2</v>
       </c>
-      <c r="D6" s="7"/>
+      <c r="D6" s="12"/>
       <c r="E6" s="1">
         <v>2.374854</v>
       </c>
-      <c r="F6" s="7"/>
+      <c r="F6" s="12"/>
       <c r="G6" s="1">
         <v>23.998033</v>
       </c>
-      <c r="H6" s="7"/>
+      <c r="H6" s="12"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6.3029999999999996E-3</v>
       </c>
-      <c r="B7" s="7"/>
+      <c r="B7" s="12"/>
       <c r="C7" s="1">
         <v>8.7035000000000001E-2</v>
       </c>
-      <c r="D7" s="7"/>
+      <c r="D7" s="12"/>
       <c r="E7" s="1">
         <v>2.3720530000000002</v>
       </c>
-      <c r="F7" s="7"/>
+      <c r="F7" s="12"/>
       <c r="G7" s="1">
         <v>23.919460000000001</v>
       </c>
-      <c r="H7" s="7"/>
+      <c r="H7" s="12"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
@@ -1500,44 +1500,44 @@
       <c r="A11" s="3">
         <v>4.3769999999999998E-3</v>
       </c>
-      <c r="B11" s="24">
+      <c r="B11" s="22">
         <f>AVERAGE(A11:A15)</f>
         <v>4.4596000000000002E-3</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="6">
         <f>B3/B11</f>
         <v>1.4573504350165931</v>
       </c>
       <c r="D11" s="3">
         <v>6.8006999999999998E-2</v>
       </c>
-      <c r="E11" s="24">
+      <c r="E11" s="22">
         <f>AVERAGE(D11:D15)</f>
         <v>6.4985799999999996E-2</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="6">
         <f>D3/E11</f>
         <v>0.75983984193469967</v>
       </c>
       <c r="G11" s="3">
         <v>6.6232480000000002</v>
       </c>
-      <c r="H11" s="24">
+      <c r="H11" s="22">
         <f>AVERAGE(G11:G15)</f>
         <v>6.686429200000001</v>
       </c>
-      <c r="I11" s="12">
+      <c r="I11" s="6">
         <f>F3/H11</f>
         <v>0.3577625558347346</v>
       </c>
       <c r="J11" s="3">
         <v>89.042483000000004</v>
       </c>
-      <c r="K11" s="24">
+      <c r="K11" s="22">
         <f>AVERAGE(J11:J15)</f>
         <v>74.137772400000017</v>
       </c>
-      <c r="L11" s="12">
+      <c r="L11" s="6">
         <f>H3/K11</f>
         <v>0.32228830765354899</v>
       </c>
@@ -1546,105 +1546,105 @@
       <c r="A12" s="3">
         <v>4.4380000000000001E-3</v>
       </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="13"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="7"/>
       <c r="D12" s="3">
         <v>4.1998000000000001E-2</v>
       </c>
-      <c r="E12" s="25"/>
-      <c r="F12" s="13"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="7"/>
       <c r="G12" s="3">
         <v>6.5891760000000001</v>
       </c>
-      <c r="H12" s="25"/>
-      <c r="I12" s="13"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="7"/>
       <c r="J12" s="3">
         <v>71.662083999999993</v>
       </c>
-      <c r="K12" s="25"/>
-      <c r="L12" s="13"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="7"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>4.5110000000000003E-3</v>
       </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="13"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="7"/>
       <c r="D13" s="3">
         <v>4.3872000000000001E-2</v>
       </c>
-      <c r="E13" s="25"/>
-      <c r="F13" s="13"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="7"/>
       <c r="G13" s="3">
         <v>6.7215730000000002</v>
       </c>
-      <c r="H13" s="25"/>
-      <c r="I13" s="13"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="7"/>
       <c r="J13" s="3">
         <v>69.002851000000007</v>
       </c>
-      <c r="K13" s="25"/>
-      <c r="L13" s="13"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="7"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>4.5250000000000004E-3</v>
       </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="13"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="7"/>
       <c r="D14" s="3">
         <v>5.8254E-2</v>
       </c>
-      <c r="E14" s="25"/>
-      <c r="F14" s="13"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="7"/>
       <c r="G14" s="3">
         <v>6.7527499999999998</v>
       </c>
-      <c r="H14" s="25"/>
-      <c r="I14" s="13"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="7"/>
       <c r="J14" s="3">
         <v>68.275855000000007</v>
       </c>
-      <c r="K14" s="25"/>
-      <c r="L14" s="13"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="7"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>4.4470000000000004E-3</v>
       </c>
-      <c r="B15" s="26"/>
-      <c r="C15" s="14"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="8"/>
       <c r="D15" s="3">
         <v>0.112798</v>
       </c>
-      <c r="E15" s="26"/>
-      <c r="F15" s="14"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="8"/>
       <c r="G15" s="3">
         <v>6.7453989999999999</v>
       </c>
-      <c r="H15" s="26"/>
-      <c r="I15" s="14"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="8"/>
       <c r="J15" s="3">
         <v>72.705589000000003</v>
       </c>
-      <c r="K15" s="26"/>
-      <c r="L15" s="14"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="8"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
@@ -1688,44 +1688,44 @@
       <c r="A19" s="3">
         <v>4.8999999999999998E-3</v>
       </c>
-      <c r="B19" s="24">
+      <c r="B19" s="22">
         <f>AVERAGE(A19:A23)</f>
         <v>4.6842000000000003E-3</v>
       </c>
-      <c r="C19" s="12">
+      <c r="C19" s="6">
         <f>B3/B19</f>
         <v>1.3874727808377094</v>
       </c>
       <c r="D19" s="3">
         <v>5.6577000000000002E-2</v>
       </c>
-      <c r="E19" s="24">
+      <c r="E19" s="22">
         <f>AVERAGE(D19:D23)</f>
         <v>4.8751799999999998E-2</v>
       </c>
-      <c r="F19" s="12">
+      <c r="F19" s="6">
         <f>D3/E19</f>
         <v>1.0128610635914983</v>
       </c>
       <c r="G19" s="3">
         <v>3.4884689999999998</v>
       </c>
-      <c r="H19" s="24">
+      <c r="H19" s="22">
         <f>AVERAGE(G19:G23)</f>
         <v>3.6097006</v>
       </c>
-      <c r="I19" s="12">
+      <c r="I19" s="6">
         <f>F3/H19</f>
         <v>0.6627014993985928</v>
       </c>
       <c r="J19" s="3">
         <v>40.36327</v>
       </c>
-      <c r="K19" s="24">
+      <c r="K19" s="22">
         <f>AVERAGE(J19:J23)</f>
         <v>41.001088199999991</v>
       </c>
-      <c r="L19" s="12">
+      <c r="L19" s="6">
         <f>H3/K19</f>
         <v>0.58275861078243296</v>
       </c>
@@ -1734,105 +1734,105 @@
       <c r="A20" s="3">
         <v>4.7720000000000002E-3</v>
       </c>
-      <c r="B20" s="25"/>
-      <c r="C20" s="13"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="7"/>
       <c r="D20" s="3">
         <v>6.0916999999999999E-2</v>
       </c>
-      <c r="E20" s="25"/>
-      <c r="F20" s="13"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="7"/>
       <c r="G20" s="3">
         <v>3.561401</v>
       </c>
-      <c r="H20" s="25"/>
-      <c r="I20" s="13"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="7"/>
       <c r="J20" s="3">
         <v>47.20411</v>
       </c>
-      <c r="K20" s="25"/>
-      <c r="L20" s="13"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="7"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>4.9020000000000001E-3</v>
       </c>
-      <c r="B21" s="25"/>
-      <c r="C21" s="13"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="7"/>
       <c r="D21" s="3">
         <v>4.2832000000000002E-2</v>
       </c>
-      <c r="E21" s="25"/>
-      <c r="F21" s="13"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="7"/>
       <c r="G21" s="3">
         <v>3.6326170000000002</v>
       </c>
-      <c r="H21" s="25"/>
-      <c r="I21" s="13"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="7"/>
       <c r="J21" s="3">
         <v>41.847327999999997</v>
       </c>
-      <c r="K21" s="25"/>
-      <c r="L21" s="13"/>
+      <c r="K21" s="23"/>
+      <c r="L21" s="7"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>4.4450000000000002E-3</v>
       </c>
-      <c r="B22" s="25"/>
-      <c r="C22" s="13"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="7"/>
       <c r="D22" s="3">
         <v>4.1216999999999997E-2</v>
       </c>
-      <c r="E22" s="25"/>
-      <c r="F22" s="13"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="7"/>
       <c r="G22" s="3">
         <v>3.6529639999999999</v>
       </c>
-      <c r="H22" s="25"/>
-      <c r="I22" s="13"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="7"/>
       <c r="J22" s="3">
         <v>37.903092999999998</v>
       </c>
-      <c r="K22" s="25"/>
-      <c r="L22" s="13"/>
+      <c r="K22" s="23"/>
+      <c r="L22" s="7"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>4.4019999999999997E-3</v>
       </c>
-      <c r="B23" s="26"/>
-      <c r="C23" s="14"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="8"/>
       <c r="D23" s="3">
         <v>4.2215999999999997E-2</v>
       </c>
-      <c r="E23" s="26"/>
-      <c r="F23" s="14"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="8"/>
       <c r="G23" s="3">
         <v>3.7130519999999998</v>
       </c>
-      <c r="H23" s="26"/>
-      <c r="I23" s="14"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="8"/>
       <c r="J23" s="3">
         <v>37.687640000000002</v>
       </c>
-      <c r="K23" s="26"/>
-      <c r="L23" s="14"/>
+      <c r="K23" s="24"/>
+      <c r="L23" s="8"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
@@ -1876,44 +1876,44 @@
       <c r="A27" s="3">
         <v>4.3699999999999998E-3</v>
       </c>
-      <c r="B27" s="24">
+      <c r="B27" s="22">
         <f>AVERAGE(A27:A31)</f>
         <v>4.3296000000000003E-3</v>
       </c>
-      <c r="C27" s="12">
+      <c r="C27" s="6">
         <f>B3/B27</f>
         <v>1.5011086474501105</v>
       </c>
       <c r="D27" s="3">
         <v>6.8677000000000002E-2</v>
       </c>
-      <c r="E27" s="24">
+      <c r="E27" s="22">
         <f>AVERAGE(D27:D31)</f>
         <v>5.2304200000000002E-2</v>
       </c>
-      <c r="F27" s="12">
+      <c r="F27" s="6">
         <f>D3/E27</f>
         <v>0.94406950111080945</v>
       </c>
       <c r="G27" s="3">
         <v>1.9634100000000001</v>
       </c>
-      <c r="H27" s="24">
+      <c r="H27" s="22">
         <f>AVERAGE(G27:G31)</f>
         <v>2.189451</v>
       </c>
-      <c r="I27" s="12">
+      <c r="I27" s="6">
         <f>F3/H27</f>
         <v>1.0925816563147566</v>
       </c>
       <c r="J27" s="3">
         <v>22.983543000000001</v>
       </c>
-      <c r="K27" s="24">
+      <c r="K27" s="22">
         <f>AVERAGE(J27:J31)</f>
         <v>24.474444599999998</v>
       </c>
-      <c r="L27" s="12">
+      <c r="L27" s="6">
         <f>H3/K27</f>
         <v>0.97627290794578447</v>
       </c>
@@ -1922,105 +1922,105 @@
       <c r="A28" s="3">
         <v>4.2700000000000004E-3</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="13"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="7"/>
       <c r="D28" s="3">
         <v>4.2324000000000001E-2</v>
       </c>
-      <c r="E28" s="25"/>
-      <c r="F28" s="13"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="7"/>
       <c r="G28" s="3">
         <v>2.1728649999999998</v>
       </c>
-      <c r="H28" s="25"/>
-      <c r="I28" s="13"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="7"/>
       <c r="J28" s="3">
         <v>23.784718999999999</v>
       </c>
-      <c r="K28" s="25"/>
-      <c r="L28" s="13"/>
+      <c r="K28" s="23"/>
+      <c r="L28" s="7"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>4.4650000000000002E-3</v>
       </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="13"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="7"/>
       <c r="D29" s="3">
         <v>4.3873000000000002E-2</v>
       </c>
-      <c r="E29" s="25"/>
-      <c r="F29" s="13"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="7"/>
       <c r="G29" s="3">
         <v>2.1944849999999998</v>
       </c>
-      <c r="H29" s="25"/>
-      <c r="I29" s="13"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="7"/>
       <c r="J29" s="3">
         <v>25.523700000000002</v>
       </c>
-      <c r="K29" s="25"/>
-      <c r="L29" s="13"/>
+      <c r="K29" s="23"/>
+      <c r="L29" s="7"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>4.3579999999999999E-3</v>
       </c>
-      <c r="B30" s="25"/>
-      <c r="C30" s="13"/>
+      <c r="B30" s="23"/>
+      <c r="C30" s="7"/>
       <c r="D30" s="3">
         <v>4.1213E-2</v>
       </c>
-      <c r="E30" s="25"/>
-      <c r="F30" s="13"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="7"/>
       <c r="G30" s="3">
         <v>2.3042750000000001</v>
       </c>
-      <c r="H30" s="25"/>
-      <c r="I30" s="13"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="7"/>
       <c r="J30" s="3">
         <v>27.042113000000001</v>
       </c>
-      <c r="K30" s="25"/>
-      <c r="L30" s="13"/>
+      <c r="K30" s="23"/>
+      <c r="L30" s="7"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>4.1850000000000004E-3</v>
       </c>
-      <c r="B31" s="26"/>
-      <c r="C31" s="14"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="8"/>
       <c r="D31" s="3">
         <v>6.5434000000000006E-2</v>
       </c>
-      <c r="E31" s="26"/>
-      <c r="F31" s="14"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="8"/>
       <c r="G31" s="3">
         <v>2.3122199999999999</v>
       </c>
-      <c r="H31" s="26"/>
-      <c r="I31" s="14"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="8"/>
       <c r="J31" s="3">
         <v>23.038148</v>
       </c>
-      <c r="K31" s="26"/>
-      <c r="L31" s="14"/>
+      <c r="K31" s="24"/>
+      <c r="L31" s="8"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
-      <c r="J33" s="5"/>
-      <c r="K33" s="5"/>
-      <c r="L33" s="5"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="10"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
@@ -2064,44 +2064,44 @@
       <c r="A35" s="3">
         <v>4.5999999999999999E-3</v>
       </c>
-      <c r="B35" s="24">
+      <c r="B35" s="22">
         <f>AVERAGE(A35:A39)</f>
         <v>5.8130000000000005E-3</v>
       </c>
-      <c r="C35" s="12">
+      <c r="C35" s="6">
         <f>B3/B35</f>
         <v>1.1180457595045585</v>
       </c>
       <c r="D35" s="3">
         <v>4.335E-2</v>
       </c>
-      <c r="E35" s="24">
+      <c r="E35" s="22">
         <f>AVERAGE(D35:D39)</f>
         <v>4.2192600000000004E-2</v>
       </c>
-      <c r="F35" s="12">
+      <c r="F35" s="6">
         <f>D3/E35</f>
         <v>1.1703189658850128</v>
       </c>
       <c r="G35" s="3">
         <v>1.668833</v>
       </c>
-      <c r="H35" s="24">
+      <c r="H35" s="22">
         <f>AVERAGE(G35:G39)</f>
         <v>1.9743895999999999</v>
       </c>
-      <c r="I35" s="12">
+      <c r="I35" s="6">
         <f>F3/H35</f>
         <v>1.2115916737000643</v>
       </c>
       <c r="J35" s="3">
         <v>21.320739</v>
       </c>
-      <c r="K35" s="24">
+      <c r="K35" s="22">
         <f>AVERAGE(J35:J39)</f>
         <v>21.781726599999999</v>
       </c>
-      <c r="L35" s="12">
+      <c r="L35" s="6">
         <f>H3/K35</f>
         <v>1.0969624969950731</v>
       </c>
@@ -2110,111 +2110,98 @@
       <c r="A36" s="3">
         <v>4.5840000000000004E-3</v>
       </c>
-      <c r="B36" s="25"/>
-      <c r="C36" s="13"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="7"/>
       <c r="D36" s="3">
         <v>4.1674000000000003E-2</v>
       </c>
-      <c r="E36" s="25"/>
-      <c r="F36" s="13"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="7"/>
       <c r="G36" s="3">
         <v>2.009665</v>
       </c>
-      <c r="H36" s="25"/>
-      <c r="I36" s="13"/>
+      <c r="H36" s="23"/>
+      <c r="I36" s="7"/>
       <c r="J36" s="3">
         <v>21.419577</v>
       </c>
-      <c r="K36" s="25"/>
-      <c r="L36" s="13"/>
+      <c r="K36" s="23"/>
+      <c r="L36" s="7"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>7.3130000000000001E-3</v>
       </c>
-      <c r="B37" s="25"/>
-      <c r="C37" s="13"/>
+      <c r="B37" s="23"/>
+      <c r="C37" s="7"/>
       <c r="D37" s="3">
         <v>4.2286999999999998E-2</v>
       </c>
-      <c r="E37" s="25"/>
-      <c r="F37" s="13"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="7"/>
       <c r="G37" s="3">
         <v>2.188358</v>
       </c>
-      <c r="H37" s="25"/>
-      <c r="I37" s="13"/>
+      <c r="H37" s="23"/>
+      <c r="I37" s="7"/>
       <c r="J37" s="3">
         <v>21.917483000000001</v>
       </c>
-      <c r="K37" s="25"/>
-      <c r="L37" s="13"/>
+      <c r="K37" s="23"/>
+      <c r="L37" s="7"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>4.6990000000000001E-3</v>
       </c>
-      <c r="B38" s="25"/>
-      <c r="C38" s="13"/>
+      <c r="B38" s="23"/>
+      <c r="C38" s="7"/>
       <c r="D38" s="3">
         <v>4.1896999999999997E-2</v>
       </c>
-      <c r="E38" s="25"/>
-      <c r="F38" s="13"/>
+      <c r="E38" s="23"/>
+      <c r="F38" s="7"/>
       <c r="G38" s="3">
         <v>2.0170970000000001</v>
       </c>
-      <c r="H38" s="25"/>
-      <c r="I38" s="13"/>
+      <c r="H38" s="23"/>
+      <c r="I38" s="7"/>
       <c r="J38" s="3">
         <v>22.68177</v>
       </c>
-      <c r="K38" s="25"/>
-      <c r="L38" s="13"/>
+      <c r="K38" s="23"/>
+      <c r="L38" s="7"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>7.8689999999999993E-3</v>
       </c>
-      <c r="B39" s="26"/>
-      <c r="C39" s="14"/>
+      <c r="B39" s="24"/>
+      <c r="C39" s="8"/>
       <c r="D39" s="3">
         <v>4.1755E-2</v>
       </c>
-      <c r="E39" s="26"/>
-      <c r="F39" s="14"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="8"/>
       <c r="G39" s="3">
         <v>1.987995</v>
       </c>
-      <c r="H39" s="26"/>
-      <c r="I39" s="14"/>
+      <c r="H39" s="24"/>
+      <c r="I39" s="8"/>
       <c r="J39" s="3">
         <v>21.569064000000001</v>
       </c>
-      <c r="K39" s="26"/>
-      <c r="L39" s="14"/>
+      <c r="K39" s="24"/>
+      <c r="L39" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="A33:L33"/>
-    <mergeCell ref="B35:B39"/>
-    <mergeCell ref="C35:C39"/>
-    <mergeCell ref="E35:E39"/>
-    <mergeCell ref="F35:F39"/>
-    <mergeCell ref="H35:H39"/>
-    <mergeCell ref="I35:I39"/>
-    <mergeCell ref="K35:K39"/>
-    <mergeCell ref="L35:L39"/>
-    <mergeCell ref="L19:L23"/>
-    <mergeCell ref="A25:L25"/>
-    <mergeCell ref="B27:B31"/>
-    <mergeCell ref="C27:C31"/>
-    <mergeCell ref="E27:E31"/>
-    <mergeCell ref="F27:F31"/>
-    <mergeCell ref="H27:H31"/>
-    <mergeCell ref="I27:I31"/>
-    <mergeCell ref="K27:K31"/>
-    <mergeCell ref="L27:L31"/>
+    <mergeCell ref="A9:L9"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="D3:D7"/>
+    <mergeCell ref="F3:F7"/>
+    <mergeCell ref="H3:H7"/>
     <mergeCell ref="K11:K15"/>
     <mergeCell ref="L11:L15"/>
     <mergeCell ref="A17:L17"/>
@@ -2231,12 +2218,25 @@
     <mergeCell ref="F11:F15"/>
     <mergeCell ref="H11:H15"/>
     <mergeCell ref="I11:I15"/>
-    <mergeCell ref="A9:L9"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="D3:D7"/>
-    <mergeCell ref="F3:F7"/>
-    <mergeCell ref="H3:H7"/>
+    <mergeCell ref="L19:L23"/>
+    <mergeCell ref="A25:L25"/>
+    <mergeCell ref="B27:B31"/>
+    <mergeCell ref="C27:C31"/>
+    <mergeCell ref="E27:E31"/>
+    <mergeCell ref="F27:F31"/>
+    <mergeCell ref="H27:H31"/>
+    <mergeCell ref="I27:I31"/>
+    <mergeCell ref="K27:K31"/>
+    <mergeCell ref="L27:L31"/>
+    <mergeCell ref="A33:L33"/>
+    <mergeCell ref="B35:B39"/>
+    <mergeCell ref="C35:C39"/>
+    <mergeCell ref="E35:E39"/>
+    <mergeCell ref="F35:F39"/>
+    <mergeCell ref="H35:H39"/>
+    <mergeCell ref="I35:I39"/>
+    <mergeCell ref="K35:K39"/>
+    <mergeCell ref="L35:L39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>